<commit_message>
fix the audio loop
</commit_message>
<xml_diff>
--- a/Noi dung may test rung - Updated.xlsx
+++ b/Noi dung may test rung - Updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\WAVGenerator\WAVGenenator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4E36AA-3B58-46AE-A8E4-33116DCCC725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ADE486-DB5F-4C14-853E-11D55139D819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58E1D11C-08BB-4978-97CC-68205073AEAB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="129">
   <si>
     <t>CHI TIẾT</t>
   </si>
@@ -368,6 +368,129 @@
 160 có nằm trong yêu cầu?
 Đề xuất: Nếu không nhập yêu cầu tăng/giảm theo giá trị, phần mềm sẽ tăng/giảm dần điều.</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>01_01</t>
+  </si>
+  <si>
+    <t>01_02</t>
+  </si>
+  <si>
+    <t>01_03</t>
+  </si>
+  <si>
+    <t>01_04</t>
+  </si>
+  <si>
+    <t>01_05</t>
+  </si>
+  <si>
+    <t>01_06</t>
+  </si>
+  <si>
+    <t>01_07</t>
+  </si>
+  <si>
+    <t>01_08</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>02_01</t>
+  </si>
+  <si>
+    <t>02_02</t>
+  </si>
+  <si>
+    <t>02_03</t>
+  </si>
+  <si>
+    <t>02_04</t>
+  </si>
+  <si>
+    <t>02_05</t>
+  </si>
+  <si>
+    <t>03_01</t>
+  </si>
+  <si>
+    <t>03_02</t>
+  </si>
+  <si>
+    <t>03_03</t>
+  </si>
+  <si>
+    <t>04_01</t>
+  </si>
+  <si>
+    <t>04_02</t>
+  </si>
+  <si>
+    <t>04_03</t>
+  </si>
+  <si>
+    <t>05_01</t>
+  </si>
+  <si>
+    <t>05_02</t>
+  </si>
+  <si>
+    <t>05_03</t>
+  </si>
+  <si>
+    <t>06_01</t>
+  </si>
+  <si>
+    <t>06_02</t>
+  </si>
+  <si>
+    <t>06_03</t>
+  </si>
+  <si>
+    <t>07_01</t>
+  </si>
+  <si>
+    <t>07_02</t>
+  </si>
+  <si>
+    <t>07_03</t>
+  </si>
+  <si>
+    <t>08_01</t>
+  </si>
+  <si>
+    <t>08_02</t>
+  </si>
+  <si>
+    <t>08_03</t>
+  </si>
+  <si>
+    <t>08_04</t>
+  </si>
+  <si>
+    <t>09_01</t>
+  </si>
+  <si>
+    <t>09_02</t>
+  </si>
+  <si>
+    <t>10_01</t>
+  </si>
+  <si>
+    <t>10_02</t>
+  </si>
+  <si>
+    <t>10_03</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
 </sst>
 </file>
 
@@ -376,7 +499,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +613,35 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +688,21 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -728,10 +893,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -782,6 +950,42 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,8 +995,41 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -807,80 +1044,39 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -906,10 +1102,10 @@
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3202305</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1875155</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>122314</xdr:rowOff>
+      <xdr:rowOff>125489</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -949,8 +1145,8 @@
       <xdr:rowOff>136524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3140710</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1819910</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>39370</xdr:rowOff>
     </xdr:to>
@@ -992,8 +1188,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3079115</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1755140</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>151527</xdr:rowOff>
     </xdr:to>
@@ -1035,8 +1231,8 @@
       <xdr:rowOff>187325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3302000</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1978025</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>96255</xdr:rowOff>
     </xdr:to>
@@ -1073,13 +1269,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3225801</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3778251</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>53975</xdr:rowOff>
@@ -1148,13 +1344,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3248026</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3800476</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
@@ -1223,13 +1419,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3187701</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3740151</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -1294,13 +1490,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3143251</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3695701</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -1663,1351 +1859,1652 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F28A2C2-5F01-4432-A991-D66E9CE3B3AE}">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="1.6328125" customWidth="1"/>
     <col min="8" max="8" width="29.1796875" customWidth="1"/>
-    <col min="9" max="9" width="54.81640625" customWidth="1"/>
-    <col min="10" max="10" width="33.453125" customWidth="1"/>
-    <col min="11" max="11" width="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="54.81640625" customWidth="1"/>
+    <col min="12" max="12" width="33.453125" customWidth="1"/>
+    <col min="13" max="13" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1">
+    <row r="1" spans="1:14" ht="21" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="36.75" customHeight="1">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="36.75" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="50"/>
+      <c r="I2" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="24">
+    <row r="3" spans="1:14" ht="24">
       <c r="A3" s="4"/>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5">
+    <row r="4" spans="1:14" ht="15.5">
       <c r="A4" s="4"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="8" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="L4" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.5">
+    <row r="5" spans="1:14" ht="15.5">
       <c r="A5" s="4"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="8" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.5">
+    <row r="6" spans="1:14" ht="15.5">
       <c r="A6" s="5"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="8" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="L6" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29.4" customHeight="1">
+    <row r="7" spans="1:14">
       <c r="A7" s="3"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="35" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="L7" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="M7" s="52" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="20.5" customHeight="1">
+      <c r="N7" s="24"/>
+    </row>
+    <row r="8" spans="1:14" ht="24.5" customHeight="1">
       <c r="A8" s="3"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" ht="23" customHeight="1">
+      <c r="B8" s="42"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" ht="26" customHeight="1">
       <c r="A9" s="3"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.5">
+      <c r="B9" s="42"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.5">
       <c r="A10" s="3"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="34"/>
+      <c r="I10" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="L10" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.5">
+    <row r="11" spans="1:14" ht="36" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="8" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="24">
+    <row r="12" spans="1:14" ht="36" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.5">
+    <row r="13" spans="1:14" ht="15.5">
       <c r="A13" s="3"/>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="8" t="s">
+      <c r="H13" s="34"/>
+      <c r="I13" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="L13" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="21.65" customHeight="1">
+    <row r="14" spans="1:14" ht="21.65" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="6" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="L14" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="24">
+    <row r="15" spans="1:14" ht="24">
       <c r="A15" s="3"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="7" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J15" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="L15" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="24">
+    <row r="16" spans="1:14" ht="24">
       <c r="A16" s="3"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="L16" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="24">
+    <row r="17" spans="1:13" ht="24">
       <c r="A17" s="3"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="L17" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="24">
+    <row r="18" spans="1:13" ht="24">
       <c r="A18" s="3"/>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="L18" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="24">
+    <row r="19" spans="1:13" ht="24">
       <c r="A19" s="3"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="L19" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.75" customHeight="1">
+    <row r="20" spans="1:13" ht="28.75" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="7" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="L20" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="M20" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.5">
+    <row r="21" spans="1:13" ht="15.5">
       <c r="A21" s="3"/>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21" t="s">
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="8" t="s">
+      <c r="H21" s="34"/>
+      <c r="I21" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J21" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="L21" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.5">
+    <row r="22" spans="1:13" ht="15.5">
       <c r="A22" s="3"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="8" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="L22" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.5">
+    <row r="23" spans="1:13" ht="15.5">
       <c r="A23" s="3"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="8" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="L23" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.5">
+    <row r="24" spans="1:13" ht="15.5">
       <c r="A24" s="3"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21" t="s">
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="8" t="s">
+      <c r="H24" s="34"/>
+      <c r="I24" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="L24" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.5">
+    <row r="25" spans="1:13" ht="15.5">
       <c r="A25" s="3"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="8" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="L25" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.5">
+    <row r="26" spans="1:13" ht="15.5">
       <c r="A26" s="3"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="6" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="16" t="s">
+      <c r="L26" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.5">
+    <row r="27" spans="1:13" ht="15.5">
       <c r="A27" s="3"/>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21" t="s">
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="8" t="s">
+      <c r="H27" s="34"/>
+      <c r="I27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="L27" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.5">
+    <row r="28" spans="1:13" ht="15.5">
       <c r="A28" s="3"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="8" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="J28" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K28" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="L28" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:13">
       <c r="A29" s="3"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" ht="24" customHeight="1">
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:13" ht="24" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21" t="s">
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="34"/>
       <c r="I30" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="16" t="s">
+      <c r="L30" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1">
+    <row r="31" spans="1:13" ht="21" customHeight="1">
       <c r="A31" s="3"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="8" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="L31" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1">
+    <row r="32" spans="1:13" ht="21" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="8" t="s">
+      <c r="B32" s="32"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" s="10"/>
+      <c r="K32" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J32" s="16" t="s">
+      <c r="L32" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="21" customHeight="1">
+    <row r="33" spans="1:12" ht="21" customHeight="1">
       <c r="A33" s="3"/>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21" t="s">
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="8" t="s">
+      <c r="H33" s="34"/>
+      <c r="I33" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="J33" s="10"/>
+      <c r="K33" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J33" s="16" t="s">
+      <c r="L33" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="21" customHeight="1">
+    <row r="34" spans="1:12" ht="21" customHeight="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="8" t="s">
+      <c r="B34" s="32"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J34" s="10"/>
+      <c r="K34" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="L34" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="21" customHeight="1">
+    <row r="35" spans="1:12" ht="21" customHeight="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="8" t="s">
+      <c r="B35" s="32"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="L35" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="21" customHeight="1">
+    <row r="36" spans="1:12" ht="21" customHeight="1">
       <c r="A36" s="3"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="8" t="s">
+      <c r="B36" s="32"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="10"/>
+      <c r="K36" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="L36" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="21" customHeight="1">
+    <row r="37" spans="1:12" ht="21" customHeight="1">
       <c r="A37" s="3"/>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21" t="s">
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="8" t="s">
+      <c r="H37" s="34"/>
+      <c r="I37" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="L37" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="21" customHeight="1">
+    <row r="38" spans="1:12" ht="21" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="8" t="s">
+      <c r="B38" s="32"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J38" s="10"/>
+      <c r="K38" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="L38" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="21" customHeight="1">
+    <row r="39" spans="1:12" ht="21" customHeight="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" ht="21" customHeight="1">
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:12" ht="21" customHeight="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="1:10" ht="21" customHeight="1">
+      <c r="B40" s="32"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="1:12" ht="21" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21" t="s">
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="8" t="s">
+      <c r="H41" s="34"/>
+      <c r="I41" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J41" s="10"/>
+      <c r="K41" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="L41" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="21" customHeight="1">
+    <row r="42" spans="1:12" ht="21" customHeight="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="8" t="s">
+      <c r="B42" s="32"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J42" s="10"/>
+      <c r="K42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="L42" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="21" customHeight="1">
+    <row r="43" spans="1:12" ht="21" customHeight="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="8" t="s">
+      <c r="B43" s="32"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="J43" s="10"/>
+      <c r="K43" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="L43" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:12">
       <c r="C45" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:12">
       <c r="D46" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:12">
       <c r="D47" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="2:10">
-      <c r="B49" s="50" t="s">
+    <row r="49" spans="2:12">
+      <c r="B49" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="12" t="s">
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:10">
-      <c r="B50" s="38"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="29" t="s">
+    <row r="50" spans="2:12">
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B51" s="41"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="30"/>
-    </row>
-    <row r="52" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B52" s="41"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="30"/>
-    </row>
-    <row r="53" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B53" s="41"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="30"/>
-    </row>
-    <row r="54" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B54" s="41"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="30"/>
-    </row>
-    <row r="55" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B55" s="41"/>
-      <c r="C55" s="42"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="30"/>
-    </row>
-    <row r="56" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B56" s="41"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="30"/>
-    </row>
-    <row r="57" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B57" s="41"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="42"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="30"/>
-    </row>
-    <row r="58" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B58" s="41"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
-      <c r="I58" s="43"/>
-      <c r="J58" s="30"/>
-    </row>
-    <row r="59" spans="2:10">
-      <c r="B59" s="44"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="31"/>
-    </row>
-    <row r="60" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B60" s="38"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="29" t="s">
+    <row r="51" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B51" s="23"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="27"/>
+    </row>
+    <row r="52" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B52" s="23"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="27"/>
+    </row>
+    <row r="53" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="27"/>
+    </row>
+    <row r="54" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B54" s="23"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="27"/>
+    </row>
+    <row r="55" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B55" s="23"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="27"/>
+    </row>
+    <row r="56" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="27"/>
+    </row>
+    <row r="57" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B57" s="23"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="24"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="27"/>
+    </row>
+    <row r="58" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="25"/>
+      <c r="L58" s="27"/>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="36"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="28"/>
+    </row>
+    <row r="60" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B60" s="20"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B61" s="41"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="43"/>
-      <c r="J61" s="30"/>
-    </row>
-    <row r="62" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B62" s="41"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="30"/>
-    </row>
-    <row r="63" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B63" s="41"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="30"/>
-    </row>
-    <row r="64" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B64" s="41"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="30"/>
-    </row>
-    <row r="65" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B65" s="41"/>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="30"/>
-    </row>
-    <row r="66" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B66" s="41"/>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="30"/>
-    </row>
-    <row r="67" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B67" s="41"/>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="43"/>
-      <c r="J67" s="30"/>
-    </row>
-    <row r="68" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B68" s="41"/>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="43"/>
-      <c r="J68" s="30"/>
-    </row>
-    <row r="69" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B69" s="41"/>
-      <c r="C69" s="42"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="42"/>
-      <c r="F69" s="42"/>
-      <c r="G69" s="42"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="30"/>
-    </row>
-    <row r="70" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B70" s="41"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="31"/>
-    </row>
-    <row r="71" spans="2:10">
-      <c r="B71" s="38"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="40"/>
-      <c r="J71" s="29" t="s">
+    <row r="61" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B61" s="23"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+      <c r="J61" s="24"/>
+      <c r="K61" s="25"/>
+      <c r="L61" s="27"/>
+    </row>
+    <row r="62" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="27"/>
+    </row>
+    <row r="63" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="25"/>
+      <c r="L63" s="27"/>
+    </row>
+    <row r="64" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="24"/>
+      <c r="J64" s="24"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="27"/>
+    </row>
+    <row r="65" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B65" s="23"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+      <c r="J65" s="24"/>
+      <c r="K65" s="25"/>
+      <c r="L65" s="27"/>
+    </row>
+    <row r="66" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B66" s="23"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="25"/>
+      <c r="L66" s="27"/>
+    </row>
+    <row r="67" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B67" s="23"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="25"/>
+      <c r="L67" s="27"/>
+    </row>
+    <row r="68" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B68" s="23"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="24"/>
+      <c r="J68" s="24"/>
+      <c r="K68" s="25"/>
+      <c r="L68" s="27"/>
+    </row>
+    <row r="69" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B69" s="23"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="24"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="27"/>
+    </row>
+    <row r="70" spans="2:12" ht="15.5" customHeight="1">
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="25"/>
+      <c r="L70" s="28"/>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B72" s="41"/>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="42"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="30"/>
-    </row>
-    <row r="73" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B73" s="41"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="42"/>
-      <c r="F73" s="42"/>
-      <c r="G73" s="42"/>
-      <c r="H73" s="42"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="30"/>
-    </row>
-    <row r="74" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B74" s="41"/>
-      <c r="C74" s="42"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="42"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="42"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="43"/>
-      <c r="J74" s="30"/>
-    </row>
-    <row r="75" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B75" s="41"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42"/>
-      <c r="F75" s="42"/>
-      <c r="G75" s="42"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="43"/>
-      <c r="J75" s="30"/>
-    </row>
-    <row r="76" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B76" s="41"/>
-      <c r="C76" s="42"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="42"/>
-      <c r="F76" s="42"/>
-      <c r="G76" s="42"/>
-      <c r="H76" s="42"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="30"/>
-    </row>
-    <row r="77" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B77" s="41"/>
-      <c r="C77" s="42"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="42"/>
-      <c r="F77" s="42"/>
-      <c r="G77" s="42"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="30"/>
-    </row>
-    <row r="78" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B78" s="41"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="42"/>
-      <c r="F78" s="42"/>
-      <c r="G78" s="42"/>
-      <c r="H78" s="42"/>
-      <c r="I78" s="43"/>
-      <c r="J78" s="30"/>
-    </row>
-    <row r="79" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B79" s="41"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="42"/>
-      <c r="F79" s="42"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="30"/>
-    </row>
-    <row r="80" spans="2:10">
-      <c r="B80" s="41"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="43"/>
-      <c r="J80" s="30"/>
-    </row>
-    <row r="81" spans="2:10">
-      <c r="B81" s="41"/>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
-      <c r="F81" s="42"/>
-      <c r="G81" s="42"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="43"/>
-      <c r="J81" s="30"/>
-    </row>
-    <row r="82" spans="2:10">
-      <c r="B82" s="44"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="45"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="46"/>
-      <c r="J82" s="31"/>
-    </row>
-    <row r="83" spans="2:10">
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="39"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="29" t="s">
+    <row r="72" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B72" s="23"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="25"/>
+      <c r="L72" s="27"/>
+    </row>
+    <row r="73" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B73" s="23"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="25"/>
+      <c r="L73" s="27"/>
+    </row>
+    <row r="74" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B74" s="23"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="25"/>
+      <c r="L74" s="27"/>
+    </row>
+    <row r="75" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B75" s="23"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="25"/>
+      <c r="L75" s="27"/>
+    </row>
+    <row r="76" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B76" s="23"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="25"/>
+      <c r="L76" s="27"/>
+    </row>
+    <row r="77" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="25"/>
+      <c r="L77" s="27"/>
+    </row>
+    <row r="78" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B78" s="23"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="25"/>
+      <c r="L78" s="27"/>
+    </row>
+    <row r="79" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B79" s="23"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="25"/>
+      <c r="L79" s="27"/>
+    </row>
+    <row r="80" spans="2:12">
+      <c r="B80" s="23"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="25"/>
+      <c r="L80" s="27"/>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="23"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="25"/>
+      <c r="L81" s="27"/>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="B82" s="35"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="28"/>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="B83" s="20"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="K83" s="22"/>
+      <c r="L83" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B84" s="41"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
-      <c r="F84" s="42"/>
-      <c r="G84" s="42"/>
-      <c r="H84" s="42"/>
-      <c r="I84" s="43"/>
-      <c r="J84" s="30"/>
-    </row>
-    <row r="85" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B85" s="41"/>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
-      <c r="F85" s="42"/>
-      <c r="G85" s="42"/>
-      <c r="H85" s="42"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="30"/>
-    </row>
-    <row r="86" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B86" s="41"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="42"/>
-      <c r="F86" s="42"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="42"/>
-      <c r="I86" s="43"/>
-      <c r="J86" s="30"/>
-    </row>
-    <row r="87" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B87" s="41"/>
-      <c r="C87" s="42"/>
-      <c r="D87" s="42"/>
-      <c r="E87" s="42"/>
-      <c r="F87" s="42"/>
-      <c r="G87" s="42"/>
-      <c r="H87" s="42"/>
-      <c r="I87" s="43"/>
-      <c r="J87" s="30"/>
-    </row>
-    <row r="88" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B88" s="41"/>
-      <c r="C88" s="42"/>
-      <c r="D88" s="42"/>
-      <c r="E88" s="42"/>
-      <c r="F88" s="42"/>
-      <c r="G88" s="42"/>
-      <c r="H88" s="42"/>
-      <c r="I88" s="43"/>
-      <c r="J88" s="30"/>
-    </row>
-    <row r="89" spans="2:10" ht="14.4" customHeight="1">
-      <c r="B89" s="41"/>
-      <c r="C89" s="42"/>
-      <c r="D89" s="42"/>
-      <c r="E89" s="42"/>
-      <c r="F89" s="42"/>
-      <c r="G89" s="42"/>
-      <c r="H89" s="42"/>
-      <c r="I89" s="43"/>
-      <c r="J89" s="30"/>
-    </row>
-    <row r="90" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B90" s="41"/>
-      <c r="C90" s="42"/>
-      <c r="D90" s="42"/>
-      <c r="E90" s="42"/>
-      <c r="F90" s="42"/>
-      <c r="G90" s="42"/>
-      <c r="H90" s="42"/>
-      <c r="I90" s="43"/>
-      <c r="J90" s="30"/>
-    </row>
-    <row r="91" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B91" s="41"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="42"/>
-      <c r="E91" s="42"/>
-      <c r="F91" s="42"/>
-      <c r="G91" s="42"/>
-      <c r="H91" s="42"/>
-      <c r="I91" s="43"/>
-      <c r="J91" s="30"/>
-    </row>
-    <row r="92" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B92" s="41"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="42"/>
-      <c r="F92" s="42"/>
-      <c r="G92" s="42"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="43"/>
-      <c r="J92" s="30"/>
-    </row>
-    <row r="93" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B93" s="41"/>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="42"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="43"/>
-      <c r="J93" s="30"/>
-    </row>
-    <row r="94" spans="2:10" ht="14.5" customHeight="1">
-      <c r="B94" s="41"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="43"/>
-      <c r="J94" s="30"/>
-    </row>
-    <row r="95" spans="2:10">
-      <c r="B95" s="41"/>
-      <c r="C95" s="42"/>
-      <c r="D95" s="42"/>
-      <c r="E95" s="42"/>
-      <c r="F95" s="42"/>
-      <c r="G95" s="42"/>
-      <c r="H95" s="42"/>
-      <c r="I95" s="43"/>
-      <c r="J95" s="30"/>
-    </row>
-    <row r="96" spans="2:10">
-      <c r="B96" s="41"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="42"/>
-      <c r="E96" s="42"/>
-      <c r="F96" s="42"/>
-      <c r="G96" s="42"/>
-      <c r="H96" s="42"/>
-      <c r="I96" s="43"/>
-      <c r="J96" s="30"/>
-    </row>
-    <row r="97" spans="2:10">
-      <c r="B97" s="44"/>
-      <c r="C97" s="45"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="46"/>
-      <c r="J97" s="31"/>
+    <row r="84" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B84" s="23"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="27"/>
+    </row>
+    <row r="85" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B85" s="23"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="27"/>
+    </row>
+    <row r="86" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B86" s="23"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="27"/>
+    </row>
+    <row r="87" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B87" s="23"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
+      <c r="K87" s="25"/>
+      <c r="L87" s="27"/>
+    </row>
+    <row r="88" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B88" s="23"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="27"/>
+    </row>
+    <row r="89" spans="2:12" ht="14.4" customHeight="1">
+      <c r="B89" s="23"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="25"/>
+      <c r="L89" s="27"/>
+    </row>
+    <row r="90" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B90" s="23"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="25"/>
+      <c r="L90" s="27"/>
+    </row>
+    <row r="91" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B91" s="23"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="25"/>
+      <c r="L91" s="27"/>
+    </row>
+    <row r="92" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B92" s="23"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="25"/>
+      <c r="L92" s="27"/>
+    </row>
+    <row r="93" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B93" s="23"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="24"/>
+      <c r="K93" s="25"/>
+      <c r="L93" s="27"/>
+    </row>
+    <row r="94" spans="2:12" ht="14.5" customHeight="1">
+      <c r="B94" s="23"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="24"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="27"/>
+    </row>
+    <row r="95" spans="2:12">
+      <c r="B95" s="23"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="25"/>
+      <c r="L95" s="27"/>
+    </row>
+    <row r="96" spans="2:12">
+      <c r="B96" s="23"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="25"/>
+      <c r="L96" s="27"/>
+    </row>
+    <row r="97" spans="2:12">
+      <c r="B97" s="35"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="36"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="36"/>
+      <c r="I97" s="36"/>
+      <c r="J97" s="36"/>
+      <c r="K97" s="37"/>
+      <c r="L97" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="B60:I70"/>
-    <mergeCell ref="J60:J70"/>
-    <mergeCell ref="J71:J82"/>
+  <mergeCells count="50">
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="I7:I9"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:F32"/>
-    <mergeCell ref="G30:H32"/>
-    <mergeCell ref="B71:I82"/>
-    <mergeCell ref="B50:I59"/>
-    <mergeCell ref="C41:F43"/>
-    <mergeCell ref="G41:H43"/>
-    <mergeCell ref="B49:I49"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:F29"/>
-    <mergeCell ref="G27:H29"/>
-    <mergeCell ref="J83:J97"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:F36"/>
+    <mergeCell ref="G33:H36"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="G3:H9"/>
+    <mergeCell ref="C3:F9"/>
+    <mergeCell ref="C21:F23"/>
+    <mergeCell ref="G21:H23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C10:F12"/>
+    <mergeCell ref="G10:H12"/>
+    <mergeCell ref="L83:L97"/>
     <mergeCell ref="B3:B12"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="C13:F17"/>
@@ -3018,27 +3515,29 @@
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:F40"/>
     <mergeCell ref="G37:H40"/>
-    <mergeCell ref="J50:J59"/>
-    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="L50:L59"/>
+    <mergeCell ref="K7:K9"/>
     <mergeCell ref="C24:F26"/>
     <mergeCell ref="G24:H26"/>
-    <mergeCell ref="B83:I97"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="G3:H9"/>
-    <mergeCell ref="C3:F9"/>
-    <mergeCell ref="C21:F23"/>
-    <mergeCell ref="G21:H23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C10:F12"/>
-    <mergeCell ref="G10:H12"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:F36"/>
-    <mergeCell ref="G33:H36"/>
-    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="B83:K97"/>
+    <mergeCell ref="B60:K70"/>
+    <mergeCell ref="L60:L70"/>
+    <mergeCell ref="L71:L82"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:F32"/>
+    <mergeCell ref="G30:H32"/>
+    <mergeCell ref="B71:K82"/>
+    <mergeCell ref="B50:K59"/>
+    <mergeCell ref="C41:F43"/>
+    <mergeCell ref="G41:H43"/>
+    <mergeCell ref="B49:K49"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:F29"/>
+    <mergeCell ref="G27:H29"/>
   </mergeCells>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>